<commit_message>
Update test_structures_files.py with correct number of warnings and updated warning messages
</commit_message>
<xml_diff>
--- a/input_data/data_errors_3/cenarios.xlsx
+++ b/input_data/data_errors_3/cenarios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">nome</t>
   </si>
@@ -31,25 +31,10 @@
     <t xml:space="preserve">simbolo</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Otimista</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">|</t>
-    </r>
+    <t xml:space="preserve">COLUNA _A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otimista|</t>
   </si>
   <si>
     <t xml:space="preserve">Este cenário representa uma visão mais 
@@ -62,36 +47,8 @@
     <t xml:space="preserve">Pessimista</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Este cenário representa uma visão mais 
-otimista, sendo </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">|</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">baseado em um menor crescimento populacional, menor desmatamento, menor consumo, etc.</t>
-    </r>
+    <t xml:space="preserve">Este cenário representa uma visão mais 
+otimista, sendo |baseado em um menor crescimento populacional, menor desmatamento, menor consumo, etc.</t>
   </si>
   <si>
     <t xml:space="preserve">P</t>
@@ -105,7 +62,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -135,12 +92,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -325,10 +276,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+      <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.43"/>
@@ -347,7 +298,9 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -364,13 +317,13 @@
     </row>
     <row r="2" s="4" customFormat="true" ht="87" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -389,13 +342,13 @@
     </row>
     <row r="3" s="4" customFormat="true" ht="87" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>

</xml_diff>